<commit_message>
added version 1 to perft_results
</commit_message>
<xml_diff>
--- a/perft_results.xlsx
+++ b/perft_results.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20417"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Magshimim\source\repos\ChessApp\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D52957C4-5B2C-41B2-9121-297166E420B6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="20" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>version</t>
   </si>
@@ -41,17 +47,20 @@
   </si>
   <si>
     <t>v1</t>
+  </si>
+  <si>
+    <t>v2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -59,7 +68,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -110,11 +119,19 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ערכת נושא Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -156,7 +173,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -188,9 +205,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -222,6 +257,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -397,14 +450,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -430,7 +485,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -444,16 +499,42 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>0.09</v>
+        <v>0.35</v>
       </c>
       <c r="F2">
-        <v>2.2</v>
+        <v>4.46</v>
       </c>
       <c r="G2">
-        <v>49.5</v>
+        <v>123.94</v>
       </c>
       <c r="H2">
-        <v>51.8</v>
+        <v>128.76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0.1</v>
+      </c>
+      <c r="F3">
+        <v>2.37</v>
+      </c>
+      <c r="G3">
+        <v>55.12</v>
+      </c>
+      <c r="H3">
+        <v>57.6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
v3 - added magic bitboards
</commit_message>
<xml_diff>
--- a/perft_results.xlsx
+++ b/perft_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Magshimim\source\repos\ChessApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D52957C4-5B2C-41B2-9121-297166E420B6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1121FC41-6D7B-4487-A22A-8F9CBF6EED31}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="20" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>version</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t>v2</t>
+  </si>
+  <si>
+    <t>v3</t>
   </si>
 </sst>
 </file>
@@ -451,10 +454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -537,6 +540,32 @@
         <v>57.6</v>
       </c>
     </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0.08</v>
+      </c>
+      <c r="F4">
+        <v>1.25</v>
+      </c>
+      <c r="G4">
+        <v>29.29</v>
+      </c>
+      <c r="H4">
+        <v>30.68</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>